<commit_message>
feat(robot2): add robot version 2 to the project
</commit_message>
<xml_diff>
--- a/PriceComparisonRobot/PriceComparisonRobot/report.xlsx
+++ b/PriceComparisonRobot/PriceComparisonRobot/report.xlsx
@@ -14,12 +14,247 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <x:si>
-    <x:t>Ryzen 5 7600X</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+  <x:si>
+    <x:t>http://www.alza.hu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GeForce RTX 4060</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+//&lt;![CDATA[
+va</x:t>
+  </x:si>
+  <x:si>
+    <x:t>300 termék
+Java</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SZUPER ÁR
+131 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>142 690 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SZUPER ÁR
+139 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>140 790 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SZUPER ÁR
+144 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>146 090 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>220 590 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>153 790 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>254 790 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SZUPER ÁR
+133 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LEÁRAZÁS -7 %
+1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>176 490 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SZUPER ÁR
+209 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>132 890 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>220 790 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>165 590 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>172 190 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>221 690 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>208 590 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>179 290 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>215 290 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>229 790 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>128 790 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>181 190 Ft
+Kosá</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ryzen 5 5600x</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Számítógépek
+CP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>http://amazon.co.uk</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+window.ue_i</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Results
+Check e</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MSI GeForce RTX</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£289.98
+£289
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£287.97
+£287
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£295.97
+£295
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£314.00
+£314
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£309.98
+£309
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£439.98
+£439
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>£1,099.95
+£1,09</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£900.00
+£900
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£524.93
+£524
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£299.97
+£299
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£399.98
+£399
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£287.54
+£287
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£289.99
+£289
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£379.97
+£379
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£368.99
+£368
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£314.55
+£314
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£329.00
+£329
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">£850.02
+£850
+.
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Explore XUM gam</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -370,26 +605,901 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B7"/>
+  <x:dimension ref="A1:C33"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="3" spans="1:2">
+    <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:2">
+      <x:c r="C3" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
         <x:v>1</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3">
+      <x:c r="A7" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3">
+      <x:c r="A8" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:3">
+      <x:c r="A9" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:3">
+      <x:c r="A10" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:3">
+      <x:c r="A11" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:3">
+      <x:c r="A12" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:3">
+      <x:c r="A13" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:3">
+      <x:c r="A14" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:3">
+      <x:c r="A15" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:3">
+      <x:c r="A16" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:3">
+      <x:c r="A17" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:3">
+      <x:c r="A18" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:3">
+      <x:c r="A19" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:3">
+      <x:c r="A20" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:3">
+      <x:c r="A21" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:3">
+      <x:c r="A22" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:3">
+      <x:c r="A23" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:3">
+      <x:c r="A24" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:3">
+      <x:c r="A25" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:3">
+      <x:c r="A26" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:3">
+      <x:c r="A27" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:3">
+      <x:c r="A28" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:3">
+      <x:c r="A29" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:3">
+      <x:c r="A31" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:3">
+      <x:c r="A32" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:3">
+      <x:c r="A33" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:3">
+      <x:c r="A35" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:3">
+      <x:c r="A36" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:3">
+      <x:c r="A37" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:3">
+      <x:c r="A38" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:3">
+      <x:c r="A39" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:3">
+      <x:c r="A40" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:3">
+      <x:c r="A41" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:3">
+      <x:c r="A42" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:3">
+      <x:c r="A43" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:3">
+      <x:c r="A44" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:3">
+      <x:c r="A45" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:3">
+      <x:c r="A46" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:3">
+      <x:c r="A47" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:3">
+      <x:c r="A48" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:3">
+      <x:c r="A49" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:3">
+      <x:c r="A50" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:3">
+      <x:c r="A51" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:3">
+      <x:c r="A52" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C52" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:3">
+      <x:c r="A53" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C53" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:3">
+      <x:c r="A54" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:3">
+      <x:c r="A55" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:3">
+      <x:c r="A56" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:3">
+      <x:c r="A57" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C57" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:3">
+      <x:c r="A58" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C58" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:3">
+      <x:c r="A59" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C59" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:3">
+      <x:c r="A60" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C60" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:3">
+      <x:c r="A61" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C61" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:3">
+      <x:c r="A62" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C62" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:3">
+      <x:c r="A63" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C63" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:3">
+      <x:c r="A64" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C64" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:3">
+      <x:c r="A65" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C65" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:3">
+      <x:c r="A66" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C66" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:3">
+      <x:c r="A67" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C67" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:3">
+      <x:c r="A68" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C68" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" spans="1:3">
+      <x:c r="A69" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C69" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:3">
+      <x:c r="A70" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C70" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:3">
+      <x:c r="A71" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C71" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:3">
+      <x:c r="A72" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C72" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:3">
+      <x:c r="A73" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C73" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:3">
+      <x:c r="A74" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C74" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:3">
+      <x:c r="A75" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C75" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:3">
+      <x:c r="A76" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C76" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" spans="1:3">
+      <x:c r="A77" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C77" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:3">
+      <x:c r="A78" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C78" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:3">
+      <x:c r="A79" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C79" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:3">
+      <x:c r="A81" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C81" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:3">
+      <x:c r="A82" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C82" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:3">
+      <x:c r="A83" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C83" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:3">
+      <x:c r="A84" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C84" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:3">
+      <x:c r="A85" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C85" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:3">
+      <x:c r="A86" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C86" s="0" t="s">
+        <x:v>31</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>